<commit_message>
chore: fix security vulnerability found on the csv line splitter regex
</commit_message>
<xml_diff>
--- a/apps/iaimc-backend/src/assets/data/xlsx/materials.xlsx
+++ b/apps/iaimc-backend/src/assets/data/xlsx/materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeromeAwonnisebaAkum\Documents\Igus Injection Molding Project\app\igus accelerator injection molding configurator\apps\iaimc-backend\src\assets\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3628FE87-918B-4637-8662-D7A8696BDDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AABCBE-3083-4EDE-8485-92108E41543E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CF167BD9-90E8-4E93-B28F-C148AD2B16BA}"/>
   </bookViews>
@@ -511,7 +511,7 @@
     <t>&lt; 10^10</t>
   </si>
   <si>
-    <t>x</t>
+    <t>acetaldehyde_aq_40pct:o,acetamide_aq_50pct:x,acetone:+,acetyl_chloride:x,hexachlorobenzene:x,hexachloroethane:-,hexamethylphosphoric_acid_triamide:x,caustic_potash_50pct:+,potassium_bromide_aq_10pct:+,potassium_carbonate_aq_60pct:+,potassium_chloride_aq_10pct:+,potassium_chloride_aq_90pct:+,potassium_dichromate_aq_5pct:+,potassium_nitrate_aq_10pct:+,potassium_permanganate_aq_1pct:+,potassium_sulphate_saturated_solution:+,casein:x,caustic_potash_lye_aq_40pct:x,caustic_sodium_bicarb_aq_50pct:x,ketones_aliphatic:x,hydrofluorosilicic_acid_aq_30pct:+,cobalt_salts_aq:x,carbon_dioxide_gas:+,carbonic_acid_ammonia_aq_10pct:x,carbon_bisulphide:x,ozone:o,palmitic_acid:+,paraffin:+,paraffin_oil:+,perfume:+,perchlorethene:o,perchloric_acid_10pct:+,phenol_spirituous_70pct:+,phenol_aq_6pct:x,phenol_aq_88pct:+,phosphoric_acid_aq_0.3pct:+,phosphoric_acid_aq_3pct:+,phosphoric_acid_aq_10pct:+,phthalic_acid_saturated_solution:+,polyester_resins_with_styrene:x,propane_propene:+,propanol:+,propenoic_acid:x,pyridine:o,mercury:+,mercury_chloride_6pct:+,resorcinol_1.3-dihydroxybenzene_50pct:x,salicylic_acid:+,soda_solution_10pct:+,edible_fat_100pct:+,edible_oils:+,nitrogen_oxides_dry:-,styrol:o,tallow:+,tar:+,tetrahydrofuran_solvent:o,tetralin:-,white_spirit:x,xylol:-,zinc_chloride_aq_10pct:+,zinc_oxide:x,zinc_sulphate_aq_10pct:+,citric_acid_concentrated_solution:+,citric_acid_aq_10pct:+,citrus_fruits:+</t>
   </si>
 </sst>
 </file>
@@ -1375,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2C7819-D156-4459-BBA4-D3C3D4C7096B}">
   <dimension ref="A1:AO31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>